<commit_message>
Integrate db, create product & user models, create getProducts, createProduct, loginUser, registerUser routes
</commit_message>
<xml_diff>
--- a/Schema.xlsx
+++ b/Schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed\Desktop\RN\Projects\ecommerce-server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEF4419-E56D-43CD-BD05-2ADB0703F6F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB032DC2-BFB4-473C-9C9A-6D0F7C9163AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -465,9 +465,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -477,14 +474,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -495,11 +486,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -589,12 +589,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -629,6 +623,51 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
@@ -638,78 +677,39 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -732,7 +732,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CA0E380-0AA0-48D2-A729-2DDDD0030EDC}" name="Table1" displayName="Table1" ref="A2:D17" totalsRowShown="0" headerRowDxfId="51" dataDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CA0E380-0AA0-48D2-A729-2DDDD0030EDC}" name="Table1" displayName="Table1" ref="A2:D17" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="A2:D17" xr:uid="{3CA0E380-0AA0-48D2-A729-2DDDD0030EDC}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -740,17 +740,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{56CBA9F9-D97F-4CE4-AB58-0F4FE015310E}" name="Document" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{D0771108-51B0-4B6B-B36D-420F2C72A38A}" name="Type" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{C88622A0-1302-40D5-8ED1-1D9E74CF9A8C}" name="Ref" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{E6133EB3-5430-44D2-955E-E18ADFE7FC19}" name="Default" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{56CBA9F9-D97F-4CE4-AB58-0F4FE015310E}" name="Document" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{D0771108-51B0-4B6B-B36D-420F2C72A38A}" name="Type" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{C88622A0-1302-40D5-8ED1-1D9E74CF9A8C}" name="Ref" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{E6133EB3-5430-44D2-955E-E18ADFE7FC19}" name="Default" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{876CB652-9269-4DF9-893F-BA74FA31C07D}" name="Table2" displayName="Table2" ref="G2:J6" totalsRowShown="0" headerRowDxfId="42" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{876CB652-9269-4DF9-893F-BA74FA31C07D}" name="Table2" displayName="Table2" ref="G2:J6" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="G2:J6" xr:uid="{876CB652-9269-4DF9-893F-BA74FA31C07D}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -758,45 +758,45 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{93EE8691-42FC-43C2-8411-F89CFE777C79}" name="Document" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{E681D16F-17A9-4BD4-BB8B-96F250DF4B76}" name="Type" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{C73A97C3-17EB-45D2-8099-B9AB89AC7081}" name="Ref" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{803C66E9-DE47-47F6-A72F-4768BE2CE777}" name="Default" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{93EE8691-42FC-43C2-8411-F89CFE777C79}" name="Document" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{E681D16F-17A9-4BD4-BB8B-96F250DF4B76}" name="Type" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{C73A97C3-17EB-45D2-8099-B9AB89AC7081}" name="Ref" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{803C66E9-DE47-47F6-A72F-4768BE2CE777}" name="Default" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5666300D-493E-4541-8C28-569068743DB8}" name="Table14" displayName="Table14" ref="A2:F8" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5666300D-493E-4541-8C28-569068743DB8}" name="Table14" displayName="Table14" ref="A2:F8" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E842DDFA-5974-4FF2-8F20-CB6A0E74ADF4}" name="Document" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{F4429AA3-FDBD-42F5-94D7-FF655CE514EB}" name="Type" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{45ED1602-C9C1-435A-A57E-7229C51F75B5}" name="Ref" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{BD517A3F-E2E7-413B-88C9-98DF8F61A391}" name="Default" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{017729DB-A50A-4B85-8317-1CBFA84D01AC}" name="unique" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{68E235DD-7887-4534-98A9-BB12DC8852C6}" name="required" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{E842DDFA-5974-4FF2-8F20-CB6A0E74ADF4}" name="Document" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{F4429AA3-FDBD-42F5-94D7-FF655CE514EB}" name="Type" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{45ED1602-C9C1-435A-A57E-7229C51F75B5}" name="Ref" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{BD517A3F-E2E7-413B-88C9-98DF8F61A391}" name="Default" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{017729DB-A50A-4B85-8317-1CBFA84D01AC}" name="unique" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{68E235DD-7887-4534-98A9-BB12DC8852C6}" name="required" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A07B5EA-26C1-4A4C-9FA2-DC51627BF560}" name="Table145" displayName="Table145" ref="A2:F15" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A07B5EA-26C1-4A4C-9FA2-DC51627BF560}" name="Table145" displayName="Table145" ref="A2:F15" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{4E496AA3-DCBD-4FA9-BFBC-CB26F77E2EBC}" name="Document" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{E9471FE4-E554-49BB-BEC2-B590B7016D5C}" name="Type" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{64010C02-3812-45CC-945B-7215B3A278B5}" name="Ref" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{37651F5B-A059-4754-AA8C-5E102E8A5BCF}" name="Default" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{4A59242A-420F-4F49-B638-25128E22D6FF}" name="unique" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{81DA0CDC-CB20-4884-9261-F0F95B57071C}" name="required" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{4E496AA3-DCBD-4FA9-BFBC-CB26F77E2EBC}" name="Document" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{E9471FE4-E554-49BB-BEC2-B590B7016D5C}" name="Type" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{64010C02-3812-45CC-945B-7215B3A278B5}" name="Ref" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{37651F5B-A059-4754-AA8C-5E102E8A5BCF}" name="Default" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{4A59242A-420F-4F49-B638-25128E22D6FF}" name="unique" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{81DA0CDC-CB20-4884-9261-F0F95B57071C}" name="required" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B587CFB5-3F29-44BC-9942-A7E7C8AB868C}" name="Table5" displayName="Table5" ref="A18:F24" totalsRowShown="0" headerRowDxfId="16" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B587CFB5-3F29-44BC-9942-A7E7C8AB868C}" name="Table5" displayName="Table5" ref="A18:F24" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A18:F24" xr:uid="{B587CFB5-3F29-44BC-9942-A7E7C8AB868C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -806,12 +806,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{CDD1F029-4A47-40EA-8216-B9A4618D9147}" name="Document" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{AE4E3678-195E-43E8-86E8-C3FC28714C0F}" name="Type" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{889AE998-26FD-4754-B698-FFC2474B566D}" name="Ref" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{FE5A63AE-2B6E-4BC2-8545-94B2600B8E9B}" name="Default" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{75B6F0DA-7B63-4646-A91C-04F4C5983D5A}" name="unique" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{294DA7F9-35F6-46FD-868F-C12F9910BD17}" name="required" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{CDD1F029-4A47-40EA-8216-B9A4618D9147}" name="Document" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{AE4E3678-195E-43E8-86E8-C3FC28714C0F}" name="Type" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{889AE998-26FD-4754-B698-FFC2474B566D}" name="Ref" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{FE5A63AE-2B6E-4BC2-8545-94B2600B8E9B}" name="Default" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{75B6F0DA-7B63-4646-A91C-04F4C5983D5A}" name="unique" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{294DA7F9-35F6-46FD-868F-C12F9910BD17}" name="required" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1401,18 +1401,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="G1" s="15" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="G1" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1441,7 +1441,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1461,7 +1461,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1479,7 +1479,7 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1497,7 +1497,7 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1511,13 +1511,13 @@
       <c r="H6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1533,7 +1533,7 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1547,7 +1547,7 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1561,7 +1561,7 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1571,7 +1571,7 @@
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1581,7 +1581,7 @@
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1591,7 +1591,7 @@
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1603,7 +1603,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="1"/>
@@ -1613,7 +1613,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="1"/>
@@ -1623,23 +1623,23 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="1"/>
@@ -1676,14 +1676,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1706,7 +1706,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1718,7 +1718,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1730,7 +1730,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1738,13 +1738,13 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="11" t="s">
         <v>61</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1756,7 +1756,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1768,7 +1768,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1830,7 +1830,7 @@
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="6"/>
+      <c r="B16" s="5"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1838,7 +1838,7 @@
     <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="6"/>
+      <c r="C17" s="5"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
@@ -1869,14 +1869,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1899,13 +1899,13 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="1"/>
@@ -1913,24 +1913,24 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>76</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>61</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C5" s="1"/>
@@ -1939,7 +1939,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1953,7 +1953,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1967,7 +1967,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1981,7 +1981,7 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>67</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1995,7 +1995,7 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>68</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2009,7 +2009,7 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>69</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2023,7 +2023,7 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>70</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2035,7 +2035,7 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>71</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2047,7 +2047,7 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>72</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2059,10 +2059,10 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C15" s="1"/>
@@ -2071,14 +2071,14 @@
       <c r="F15" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
@@ -2101,7 +2101,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -2113,24 +2113,24 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>78</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="7"/>
+      <c r="E20" s="6"/>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="1"/>
@@ -2139,10 +2139,10 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C22" s="1"/>
@@ -2151,7 +2151,7 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2165,7 +2165,7 @@
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -2179,14 +2179,14 @@
       <c r="F24" s="1"/>
     </row>
     <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
@@ -2209,34 +2209,34 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>82</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="8"/>
+      <c r="C28" s="7"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="7"/>
+      <c r="E29" s="6"/>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C30" s="1"/>
@@ -2245,7 +2245,7 @@
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>85</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -2257,7 +2257,7 @@
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
+      <c r="A32" s="5"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2265,14 +2265,14 @@
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
@@ -2295,34 +2295,34 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="8"/>
+      <c r="C35" s="7"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="7"/>
+      <c r="E36" s="6"/>
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="1"/>

</xml_diff>